<commit_message>
Display context param validation for CaseEventtoFields tab
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V38_RDM-1202.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V38_RDM-1202.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10610"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\moj\ccd-definition-store-api\application\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedanaskhatri/project/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9C182E-CD23-444A-91C1-151A69073296}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37A41A2-15BA-5244-8E33-BF4B170152A8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1663" windowWidth="28800" windowHeight="16783" tabRatio="500" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1660" windowWidth="28800" windowHeight="16780" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="320">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1006,6 +1006,21 @@
   </si>
   <si>
     <t>LegacyCase FirstName Hint Override</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>referenceCollection</t>
+  </si>
+  <si>
+    <t>Reference Collection</t>
+  </si>
+  <si>
+    <t>MaxLength: 1000</t>
+  </si>
+  <si>
+    <t>#TABLE(Title, FirstName, MiddleName)</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1032,7 @@
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1285,6 +1300,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1542,7 +1563,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1756,6 +1777,12 @@
     <xf numFmtId="49" fontId="39" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="26" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -2149,18 +2176,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.15234375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.15234375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.84375" style="1" customWidth="1"/>
-    <col min="6" max="10" width="8.84375" style="1" customWidth="1"/>
-    <col min="11" max="1025" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" style="1" customWidth="1"/>
+    <col min="6" max="10" width="8.83203125" style="1" customWidth="1"/>
+    <col min="11" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2180,7 +2207,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -2198,7 +2225,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -2220,7 +2247,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -2240,7 +2267,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="4"/>
@@ -2252,7 +2279,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="4"/>
@@ -2264,7 +2291,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8"/>
       <c r="B7" s="10"/>
       <c r="C7" s="4"/>
@@ -2276,7 +2303,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="11"/>
       <c r="B8" s="10"/>
       <c r="C8" s="4"/>
@@ -2288,7 +2315,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11"/>
       <c r="B9" s="10"/>
       <c r="C9" s="4"/>
@@ -2300,7 +2327,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8"/>
       <c r="B10" s="10"/>
       <c r="C10" s="4"/>
@@ -2312,7 +2339,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="11"/>
       <c r="B11" s="10"/>
       <c r="C11" s="4"/>
@@ -2324,7 +2351,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="11"/>
       <c r="B12" s="10"/>
       <c r="C12" s="4"/>
@@ -2336,7 +2363,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="11"/>
       <c r="B13" s="10"/>
       <c r="C13" s="4"/>
@@ -2348,7 +2375,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="4"/>
@@ -2375,19 +2402,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.4609375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.84375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.15234375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.3046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.69140625" style="1" customWidth="1"/>
-    <col min="7" max="11" width="8.84375" style="1" customWidth="1"/>
-    <col min="12" max="1025" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="27.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="11" width="8.83203125" style="1" customWidth="1"/>
+    <col min="12" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>216</v>
       </c>
@@ -2408,7 +2435,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -2429,7 +2456,7 @@
       <c r="J2" s="54"/>
       <c r="K2" s="54"/>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -2454,7 +2481,7 @@
       <c r="J3" s="55"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="56">
         <v>42736</v>
       </c>
@@ -2477,7 +2504,7 @@
       <c r="J4" s="47"/>
       <c r="K4" s="47"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="56">
         <v>42736</v>
       </c>
@@ -2500,7 +2527,7 @@
       <c r="J5" s="47"/>
       <c r="K5" s="47"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="56">
         <v>42736</v>
       </c>
@@ -2523,7 +2550,7 @@
       <c r="J6" s="47"/>
       <c r="K6" s="47"/>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="56">
         <v>42736</v>
       </c>
@@ -2546,7 +2573,7 @@
       <c r="J7" s="47"/>
       <c r="K7" s="47"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="56">
         <v>42736</v>
       </c>
@@ -2569,7 +2596,7 @@
       <c r="J8" s="47"/>
       <c r="K8" s="47"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="56">
         <v>42736</v>
       </c>
@@ -2592,7 +2619,7 @@
       <c r="J9" s="47"/>
       <c r="K9" s="47"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="47"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
@@ -2605,7 +2632,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="47"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -2618,7 +2645,7 @@
       <c r="J11" s="47"/>
       <c r="K11" s="47"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="47"/>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
@@ -2631,7 +2658,7 @@
       <c r="J12" s="47"/>
       <c r="K12" s="47"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="47"/>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -2644,7 +2671,7 @@
       <c r="J13" s="47"/>
       <c r="K13" s="47"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
       <c r="B14" s="47"/>
       <c r="C14" s="47"/>
@@ -2657,7 +2684,7 @@
       <c r="J14" s="47"/>
       <c r="K14" s="47"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="47"/>
       <c r="B15" s="47"/>
       <c r="C15" s="47"/>
@@ -2670,7 +2697,7 @@
       <c r="J15" s="47"/>
       <c r="K15" s="47"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="47"/>
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
@@ -2683,7 +2710,7 @@
       <c r="J16" s="47"/>
       <c r="K16" s="47"/>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="47"/>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -2696,7 +2723,7 @@
       <c r="J17" s="47"/>
       <c r="K17" s="47"/>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="47"/>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -2709,7 +2736,7 @@
       <c r="J18" s="47"/>
       <c r="K18" s="47"/>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="47"/>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
@@ -2739,18 +2766,18 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.84375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="57" customWidth="1"/>
-    <col min="3" max="3" width="29.84375" style="57" customWidth="1"/>
-    <col min="4" max="4" width="19.84375" style="57" customWidth="1"/>
-    <col min="5" max="5" width="20.15234375" style="57" customWidth="1"/>
-    <col min="6" max="6" width="15.3046875" style="57" customWidth="1"/>
-    <col min="7" max="1025" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="57" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="57" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="57" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="57" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="57" customWidth="1"/>
+    <col min="7" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.05" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>219</v>
       </c>
@@ -2766,7 +2793,7 @@
       <c r="E1" s="62"/>
       <c r="F1" s="62"/>
     </row>
-    <row r="2" spans="1:6" ht="43.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.15">
       <c r="A2" s="63"/>
       <c r="B2" s="63"/>
       <c r="C2" s="64" t="s">
@@ -2782,7 +2809,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="65" t="s">
         <v>7</v>
       </c>
@@ -2802,7 +2829,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>42736</v>
       </c>
@@ -2820,7 +2847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>42736</v>
       </c>
@@ -2838,7 +2865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>42736</v>
       </c>
@@ -2856,7 +2883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>42736</v>
       </c>
@@ -2874,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52">
         <v>42736</v>
       </c>
@@ -2892,7 +2919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52">
         <v>42736</v>
       </c>
@@ -2910,7 +2937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52">
         <v>42736</v>
       </c>
@@ -2928,7 +2955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
         <v>42736</v>
       </c>
@@ -2946,7 +2973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
         <v>42736</v>
       </c>
@@ -2964,7 +2991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <v>42736</v>
       </c>
@@ -2982,7 +3009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
         <v>42736</v>
       </c>
@@ -3000,7 +3027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
         <v>42736</v>
       </c>
@@ -3018,7 +3045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
         <v>42736</v>
       </c>
@@ -3053,20 +3080,20 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.4609375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.3046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.4609375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.3046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.69140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="11" width="8.84375" style="1" customWidth="1"/>
-    <col min="12" max="1025" width="8.84375" customWidth="1"/>
+    <col min="8" max="11" width="8.83203125" style="1" customWidth="1"/>
+    <col min="12" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>223</v>
       </c>
@@ -3087,7 +3114,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="13" t="s">
@@ -3108,7 +3135,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -3133,7 +3160,7 @@
       <c r="J3" s="55"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -3156,7 +3183,7 @@
       <c r="J4" s="47"/>
       <c r="K4" s="47"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -3179,7 +3206,7 @@
       <c r="J5" s="47"/>
       <c r="K5" s="47"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -3202,7 +3229,7 @@
       <c r="J6" s="47"/>
       <c r="K6" s="47"/>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -3225,7 +3252,7 @@
       <c r="J7" s="47"/>
       <c r="K7" s="47"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>42736</v>
       </c>
@@ -3248,7 +3275,7 @@
       <c r="J8" s="47"/>
       <c r="K8" s="47"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>42736</v>
       </c>
@@ -3271,7 +3298,7 @@
       <c r="J9" s="47"/>
       <c r="K9" s="47"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
@@ -3284,7 +3311,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="47"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52"/>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -3297,7 +3324,7 @@
       <c r="J11" s="47"/>
       <c r="K11" s="47"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52"/>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
@@ -3310,7 +3337,7 @@
       <c r="J12" s="47"/>
       <c r="K12" s="47"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -3323,7 +3350,7 @@
       <c r="J13" s="47"/>
       <c r="K13" s="47"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52"/>
       <c r="B14" s="47"/>
       <c r="C14" s="47"/>
@@ -3336,7 +3363,7 @@
       <c r="J14" s="47"/>
       <c r="K14" s="47"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52"/>
       <c r="B15" s="47"/>
       <c r="C15" s="47"/>
@@ -3349,7 +3376,7 @@
       <c r="J15" s="47"/>
       <c r="K15" s="47"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
@@ -3362,7 +3389,7 @@
       <c r="J16" s="47"/>
       <c r="K16" s="47"/>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="52"/>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -3375,7 +3402,7 @@
       <c r="J17" s="47"/>
       <c r="K17" s="47"/>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="52"/>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -3388,7 +3415,7 @@
       <c r="J18" s="47"/>
       <c r="K18" s="47"/>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="52"/>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
@@ -3415,26 +3442,26 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.84375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.84375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" style="1" customWidth="1"/>
     <col min="5" max="6" width="22" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3046875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="40.84375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="21" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.84375" style="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.84375" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.83203125" style="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>224</v>
       </c>
@@ -3458,7 +3485,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="13" t="s">
@@ -3488,11 +3515,13 @@
       <c r="K2" s="105" t="s">
         <v>271</v>
       </c>
-      <c r="L2" s="4"/>
+      <c r="L2" s="157" t="s">
+        <v>318</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -3526,11 +3555,13 @@
       <c r="K3" s="106" t="s">
         <v>268</v>
       </c>
-      <c r="L3" s="8"/>
+      <c r="L3" s="159" t="s">
+        <v>315</v>
+      </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -3564,7 +3595,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -3598,7 +3629,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -3630,7 +3661,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -3662,7 +3693,7 @@
       <c r="M7" s="101"/>
       <c r="N7" s="101"/>
     </row>
-    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>42736</v>
       </c>
@@ -3694,7 +3725,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>42736</v>
       </c>
@@ -3726,7 +3757,7 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>42736</v>
       </c>
@@ -3758,7 +3789,7 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>42736</v>
       </c>
@@ -3790,7 +3821,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>42736</v>
       </c>
@@ -3822,7 +3853,7 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>42736</v>
       </c>
@@ -3854,7 +3885,7 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>42736</v>
       </c>
@@ -3886,7 +3917,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>42736</v>
       </c>
@@ -3918,7 +3949,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>42736</v>
       </c>
@@ -3950,7 +3981,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>42736</v>
       </c>
@@ -3982,7 +4013,7 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="4"/>
@@ -3998,7 +4029,7 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="4"/>
@@ -4014,7 +4045,7 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="4"/>
@@ -4030,7 +4061,7 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="4"/>
@@ -4046,7 +4077,7 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="4"/>
@@ -4062,7 +4093,7 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="4"/>
@@ -4078,7 +4109,7 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
     </row>
-    <row r="24" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="4"/>
@@ -4094,7 +4125,7 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="4"/>
@@ -4110,7 +4141,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="4"/>
@@ -4126,7 +4157,7 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
     </row>
-    <row r="27" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="4"/>
@@ -4159,20 +4190,20 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.15234375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.84375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.3046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.4609375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.84375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.84375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.4609375" style="1" customWidth="1"/>
-    <col min="8" max="11" width="8.84375" style="1" customWidth="1"/>
-    <col min="12" max="1025" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="1" customWidth="1"/>
+    <col min="8" max="11" width="8.83203125" style="1" customWidth="1"/>
+    <col min="12" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>237</v>
       </c>
@@ -4193,7 +4224,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -4206,7 +4237,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -4231,7 +4262,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="68">
         <v>42736</v>
       </c>
@@ -4256,7 +4287,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72">
         <v>42736</v>
       </c>
@@ -4281,7 +4312,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="76">
         <v>42736</v>
       </c>
@@ -4296,7 +4327,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -4309,7 +4340,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -4322,7 +4353,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -4335,7 +4366,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -4369,18 +4400,18 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.84375" style="119" customWidth="1"/>
-    <col min="2" max="2" width="24.69140625" style="119" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" style="119" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="119" customWidth="1"/>
     <col min="3" max="3" width="30" style="119" customWidth="1"/>
-    <col min="4" max="4" width="27.15234375" style="119" customWidth="1"/>
-    <col min="5" max="5" width="23.84375" style="119" customWidth="1"/>
-    <col min="6" max="6" width="47.84375" style="119" customWidth="1"/>
-    <col min="7" max="16384" width="10.84375" style="119"/>
+    <col min="4" max="4" width="27.1640625" style="119" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" style="119" customWidth="1"/>
+    <col min="6" max="6" width="47.83203125" style="119" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="119"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.600000000000001" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="120" t="s">
         <v>294</v>
       </c>
@@ -4394,7 +4425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="148" t="s">
         <v>4</v>
       </c>
@@ -4408,7 +4439,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="149" t="s">
         <v>36</v>
       </c>
@@ -4422,7 +4453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="130" t="s">
         <v>24</v>
       </c>
@@ -4436,7 +4467,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="130" t="s">
         <v>24</v>
       </c>
@@ -4450,7 +4481,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="152" t="s">
         <v>27</v>
       </c>
@@ -4464,7 +4495,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="152" t="s">
         <v>27</v>
       </c>
@@ -4478,7 +4509,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="152" t="s">
         <v>27</v>
       </c>
@@ -4492,7 +4523,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="152" t="s">
         <v>27</v>
       </c>
@@ -4519,17 +4550,17 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.84375" style="1" customWidth="1"/>
-    <col min="5" max="250" width="14.4609375" style="1" customWidth="1"/>
-    <col min="251" max="1020" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
+    <col min="5" max="250" width="14.5" style="1" customWidth="1"/>
+    <col min="251" max="1020" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" s="134" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:250" s="134" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="125" t="s">
         <v>244</v>
       </c>
@@ -4789,7 +4820,7 @@
       <c r="IO1" s="17"/>
       <c r="IP1" s="17"/>
     </row>
-    <row r="2" spans="1:250" ht="65.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:250" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="132"/>
       <c r="B2" s="132"/>
       <c r="C2" s="133" t="s">
@@ -5047,7 +5078,7 @@
       <c r="IO2" s="17"/>
       <c r="IP2" s="113"/>
     </row>
-    <row r="3" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="129" t="s">
         <v>7</v>
       </c>
@@ -5309,7 +5340,7 @@
       <c r="IO3" s="17"/>
       <c r="IP3" s="26"/>
     </row>
-    <row r="4" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="123">
         <v>42736</v>
       </c>
@@ -5569,7 +5600,7 @@
       <c r="IO4" s="17"/>
       <c r="IP4" s="26"/>
     </row>
-    <row r="5" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="123">
         <v>42736</v>
       </c>
@@ -5829,7 +5860,7 @@
       <c r="IO5" s="17"/>
       <c r="IP5" s="26"/>
     </row>
-    <row r="6" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="123">
         <v>42736</v>
       </c>
@@ -6089,7 +6120,7 @@
       <c r="IO6" s="17"/>
       <c r="IP6" s="26"/>
     </row>
-    <row r="7" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="123">
         <v>42736</v>
       </c>
@@ -6349,7 +6380,7 @@
       <c r="IO7" s="17"/>
       <c r="IP7" s="113"/>
     </row>
-    <row r="8" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:250" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="123">
         <v>42736</v>
       </c>
@@ -6609,7 +6640,7 @@
       <c r="IO8" s="17"/>
       <c r="IP8" s="26"/>
     </row>
-    <row r="9" spans="1:250" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:250" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="123">
         <v>42736</v>
       </c>
@@ -6869,7 +6900,7 @@
       <c r="IO9" s="17"/>
       <c r="IP9" s="26"/>
     </row>
-    <row r="10" spans="1:250" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:250" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="123">
         <v>42736</v>
       </c>
@@ -7129,7 +7160,7 @@
       <c r="IO10" s="17"/>
       <c r="IP10" s="113"/>
     </row>
-    <row r="11" spans="1:250" s="134" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:250" s="134" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="123">
         <v>42736</v>
       </c>
@@ -7389,7 +7420,7 @@
       <c r="IO11" s="17"/>
       <c r="IP11" s="17"/>
     </row>
-    <row r="12" spans="1:250" s="134" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:250" s="134" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -7658,18 +7689,18 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.4609375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.3046875" style="1" customWidth="1"/>
-    <col min="7" max="1019" width="8.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
+    <col min="7" max="1019" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
         <v>257</v>
       </c>
@@ -7685,7 +7716,7 @@
       <c r="E1" s="136"/>
       <c r="F1" s="136"/>
     </row>
-    <row r="2" spans="1:6" ht="65.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="137"/>
       <c r="B2" s="137"/>
       <c r="C2" s="138" t="s">
@@ -7701,7 +7732,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="140" t="s">
         <v>7</v>
       </c>
@@ -7721,7 +7752,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="141">
         <v>42736</v>
       </c>
@@ -7739,7 +7770,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="141">
         <v>42736</v>
       </c>
@@ -7757,7 +7788,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="141">
         <v>42736</v>
       </c>
@@ -7775,7 +7806,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="141">
         <v>42736</v>
       </c>
@@ -7793,7 +7824,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="141">
         <v>42736</v>
       </c>
@@ -7811,7 +7842,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="141">
         <v>42736</v>
       </c>
@@ -7829,7 +7860,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="142">
         <v>42736</v>
       </c>
@@ -7847,7 +7878,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="142">
         <v>42736</v>
       </c>
@@ -7865,7 +7896,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="141">
         <v>42736</v>
       </c>
@@ -7883,7 +7914,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="141">
         <v>42736</v>
       </c>
@@ -7901,7 +7932,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="141">
         <v>42736</v>
       </c>
@@ -7919,7 +7950,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="141">
         <v>42736</v>
       </c>
@@ -7937,7 +7968,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="141">
         <v>42736</v>
       </c>
@@ -7955,7 +7986,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="141">
         <v>42736</v>
       </c>
@@ -7973,7 +8004,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="141">
         <v>42736</v>
       </c>
@@ -7991,7 +8022,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="141">
         <v>42736</v>
       </c>
@@ -8009,7 +8040,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="141">
         <v>42736</v>
       </c>
@@ -8027,7 +8058,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="141">
         <v>42736</v>
       </c>
@@ -8045,7 +8076,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="141">
         <v>42736</v>
       </c>
@@ -8063,7 +8094,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="141">
         <v>42736</v>
       </c>
@@ -8081,7 +8112,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="141">
         <v>42736</v>
       </c>
@@ -8099,7 +8130,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="141">
         <v>42736</v>
       </c>
@@ -8117,7 +8148,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="141">
         <v>42736</v>
       </c>
@@ -8135,7 +8166,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="141">
         <v>42736</v>
       </c>
@@ -8153,7 +8184,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="141">
         <v>42736</v>
       </c>
@@ -8171,7 +8202,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="141">
         <v>42736</v>
       </c>
@@ -8189,7 +8220,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="141">
         <v>42736</v>
       </c>
@@ -8207,7 +8238,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="141">
         <v>42736</v>
       </c>
@@ -8240,17 +8271,17 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.3046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.84375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.69140625" style="1" customWidth="1"/>
-    <col min="5" max="255" width="14.4609375" style="1" customWidth="1"/>
-    <col min="256" max="1025" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="1" customWidth="1"/>
+    <col min="5" max="255" width="14.5" style="1" customWidth="1"/>
+    <col min="256" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>259</v>
       </c>
@@ -8515,7 +8546,7 @@
       <c r="IT1" s="23"/>
       <c r="IU1" s="24"/>
     </row>
-    <row r="2" spans="1:255" ht="65.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:255" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -8780,7 +8811,7 @@
       <c r="IT2" s="17"/>
       <c r="IU2" s="26"/>
     </row>
-    <row r="3" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -9049,7 +9080,7 @@
       <c r="IT3" s="17"/>
       <c r="IU3" s="26"/>
     </row>
-    <row r="4" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="79">
         <v>42736</v>
       </c>
@@ -9316,7 +9347,7 @@
       <c r="IT4" s="17"/>
       <c r="IU4" s="26"/>
     </row>
-    <row r="5" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="79">
         <v>42736</v>
       </c>
@@ -9583,7 +9614,7 @@
       <c r="IT5" s="17"/>
       <c r="IU5" s="26"/>
     </row>
-    <row r="6" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="79">
         <v>42736</v>
       </c>
@@ -9850,7 +9881,7 @@
       <c r="IT6" s="17"/>
       <c r="IU6" s="26"/>
     </row>
-    <row r="7" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="79">
         <v>42736</v>
       </c>
@@ -10117,7 +10148,7 @@
       <c r="IT7" s="17"/>
       <c r="IU7" s="26"/>
     </row>
-    <row r="8" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="79">
         <v>42736</v>
       </c>
@@ -10384,7 +10415,7 @@
       <c r="IT8" s="17"/>
       <c r="IU8" s="26"/>
     </row>
-    <row r="9" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="79">
         <v>42736</v>
       </c>
@@ -10651,7 +10682,7 @@
       <c r="IT9" s="17"/>
       <c r="IU9" s="26"/>
     </row>
-    <row r="10" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="79">
         <v>42736</v>
       </c>
@@ -10918,7 +10949,7 @@
       <c r="IT10" s="17"/>
       <c r="IU10" s="26"/>
     </row>
-    <row r="11" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="79">
         <v>42736</v>
       </c>
@@ -11185,7 +11216,7 @@
       <c r="IT11" s="17"/>
       <c r="IU11" s="26"/>
     </row>
-    <row r="12" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="79">
         <v>42736</v>
       </c>
@@ -11452,7 +11483,7 @@
       <c r="IT12" s="17"/>
       <c r="IU12" s="26"/>
     </row>
-    <row r="13" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="79">
         <v>42736</v>
       </c>
@@ -11719,7 +11750,7 @@
       <c r="IT13" s="17"/>
       <c r="IU13" s="26"/>
     </row>
-    <row r="14" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="79">
         <v>42736</v>
       </c>
@@ -11986,7 +12017,7 @@
       <c r="IT14" s="17"/>
       <c r="IU14" s="26"/>
     </row>
-    <row r="15" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="79">
         <v>42736</v>
       </c>
@@ -12270,17 +12301,17 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.15234375" style="81" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="81" customWidth="1"/>
-    <col min="3" max="3" width="27.84375" style="81" customWidth="1"/>
-    <col min="4" max="4" width="18.69140625" style="81" customWidth="1"/>
-    <col min="5" max="255" width="14.4609375" style="81" customWidth="1"/>
-    <col min="256" max="1025" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="81" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="81" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="81" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="81" customWidth="1"/>
+    <col min="5" max="255" width="14.5" style="81" customWidth="1"/>
+    <col min="256" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="82" t="s">
         <v>262</v>
       </c>
@@ -12545,7 +12576,7 @@
       <c r="IT1" s="88"/>
       <c r="IU1" s="89"/>
     </row>
-    <row r="2" spans="1:255" ht="65.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:255" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="90"/>
       <c r="B2" s="90"/>
       <c r="C2" s="91" t="s">
@@ -12568,7 +12599,7 @@
       <c r="L2" s="92"/>
       <c r="IU2" s="93"/>
     </row>
-    <row r="3" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="94" t="s">
         <v>7</v>
       </c>
@@ -12595,7 +12626,7 @@
       <c r="L3" s="92"/>
       <c r="IU3" s="93"/>
     </row>
-    <row r="4" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="96">
         <v>42736</v>
       </c>
@@ -12620,7 +12651,7 @@
       <c r="L4" s="92"/>
       <c r="IU4" s="93"/>
     </row>
-    <row r="5" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="96">
         <v>42736</v>
       </c>
@@ -12645,7 +12676,7 @@
       <c r="L5" s="92"/>
       <c r="IU5" s="93"/>
     </row>
-    <row r="6" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="96">
         <v>42736</v>
       </c>
@@ -12670,7 +12701,7 @@
       <c r="L6" s="92"/>
       <c r="IU6" s="93"/>
     </row>
-    <row r="7" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="96">
         <v>42736</v>
       </c>
@@ -12695,7 +12726,7 @@
       <c r="L7" s="92"/>
       <c r="IU7" s="93"/>
     </row>
-    <row r="8" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="96">
         <v>42736</v>
       </c>
@@ -12720,7 +12751,7 @@
       <c r="L8" s="92"/>
       <c r="IU8" s="93"/>
     </row>
-    <row r="9" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="96">
         <v>42736</v>
       </c>
@@ -12745,7 +12776,7 @@
       <c r="L9" s="92"/>
       <c r="IU9" s="93"/>
     </row>
-    <row r="10" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="96">
         <v>42736</v>
       </c>
@@ -12770,7 +12801,7 @@
       <c r="L10" s="92"/>
       <c r="IU10" s="93"/>
     </row>
-    <row r="11" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="96">
         <v>42736</v>
       </c>
@@ -12795,7 +12826,7 @@
       <c r="L11" s="92"/>
       <c r="IU11" s="93"/>
     </row>
-    <row r="12" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="96">
         <v>42736</v>
       </c>
@@ -12820,7 +12851,7 @@
       <c r="L12" s="92"/>
       <c r="IU12" s="93"/>
     </row>
-    <row r="13" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="96">
         <v>42736</v>
       </c>
@@ -12845,7 +12876,7 @@
       <c r="L13" s="92"/>
       <c r="IU13" s="93"/>
     </row>
-    <row r="14" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="96">
         <v>42736</v>
       </c>
@@ -12870,7 +12901,7 @@
       <c r="L14" s="92"/>
       <c r="IU14" s="93"/>
     </row>
-    <row r="15" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:255" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="96">
         <v>42736</v>
       </c>
@@ -13154,22 +13185,22 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.84375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.84375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.84375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.84375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.84375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.3046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="14" width="8.84375" style="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.84375" customWidth="1"/>
+    <col min="10" max="14" width="8.83203125" style="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -13193,7 +13224,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="74.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="74" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -13223,7 +13254,7 @@
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
     </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -13257,7 +13288,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -13285,7 +13316,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -13313,7 +13344,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
       <c r="B6" s="16"/>
       <c r="C6" s="17"/>
@@ -13329,7 +13360,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9"/>
       <c r="B7" s="16"/>
       <c r="C7" s="19"/>
@@ -13345,7 +13376,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="20"/>
@@ -13361,7 +13392,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="4"/>
@@ -13377,7 +13408,7 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="4"/>
@@ -13393,7 +13424,7 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="21"/>
       <c r="B11" s="9"/>
       <c r="C11" s="4"/>
@@ -13409,7 +13440,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="21"/>
       <c r="B12" s="9"/>
       <c r="C12" s="4"/>
@@ -13425,7 +13456,7 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="21"/>
       <c r="B13" s="9"/>
       <c r="C13" s="4"/>
@@ -13441,7 +13472,7 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="21"/>
       <c r="B14" s="9"/>
       <c r="C14" s="4"/>
@@ -13457,7 +13488,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="21"/>
       <c r="B15" s="9"/>
       <c r="C15" s="4"/>
@@ -13473,7 +13504,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="21"/>
       <c r="B16" s="9"/>
       <c r="C16" s="4"/>
@@ -13489,7 +13520,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="4"/>
@@ -13516,30 +13547,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W38"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" topLeftCell="B7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.4609375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.84375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.4609375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.84375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.84375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" customWidth="1"/>
     <col min="7" max="8" width="37" style="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3046875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="1" customWidth="1"/>
-    <col min="12" max="18" width="8.84375" style="1" customWidth="1"/>
-    <col min="19" max="23" width="14.4609375" style="1" customWidth="1"/>
-    <col min="24" max="1025" width="8.84375" customWidth="1"/>
+    <col min="12" max="18" width="8.83203125" style="1" customWidth="1"/>
+    <col min="19" max="23" width="14.5" style="1" customWidth="1"/>
+    <col min="24" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -13572,7 +13603,7 @@
       <c r="V1" s="23"/>
       <c r="W1" s="24"/>
     </row>
-    <row r="2" spans="1:23" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -13615,7 +13646,7 @@
       <c r="V2" s="17"/>
       <c r="W2" s="26"/>
     </row>
-    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -13666,7 +13697,7 @@
       <c r="V3" s="17"/>
       <c r="W3" s="26"/>
     </row>
-    <row r="4" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -13705,7 +13736,7 @@
       <c r="V4" s="17"/>
       <c r="W4" s="26"/>
     </row>
-    <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -13748,7 +13779,7 @@
       <c r="V5" s="17"/>
       <c r="W5" s="26"/>
     </row>
-    <row r="6" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -13787,7 +13818,7 @@
       <c r="V6" s="17"/>
       <c r="W6" s="26"/>
     </row>
-    <row r="7" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -13824,7 +13855,7 @@
       <c r="V7" s="17"/>
       <c r="W7" s="26"/>
     </row>
-    <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="27">
         <v>42736</v>
       </c>
@@ -13861,7 +13892,7 @@
       <c r="V8" s="17"/>
       <c r="W8" s="26"/>
     </row>
-    <row r="9" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="30">
         <v>42736</v>
       </c>
@@ -13898,7 +13929,7 @@
       <c r="V9" s="17"/>
       <c r="W9" s="26"/>
     </row>
-    <row r="10" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>42736</v>
       </c>
@@ -13935,7 +13966,7 @@
       <c r="V10" s="17"/>
       <c r="W10" s="26"/>
     </row>
-    <row r="11" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>42736</v>
       </c>
@@ -13972,7 +14003,7 @@
       <c r="V11" s="17"/>
       <c r="W11" s="26"/>
     </row>
-    <row r="12" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>42736</v>
       </c>
@@ -14009,7 +14040,7 @@
       <c r="V12" s="17"/>
       <c r="W12" s="26"/>
     </row>
-    <row r="13" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>42736</v>
       </c>
@@ -14046,7 +14077,7 @@
       <c r="V13" s="17"/>
       <c r="W13" s="26"/>
     </row>
-    <row r="14" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="114">
         <v>42736</v>
       </c>
@@ -14083,7 +14114,7 @@
       <c r="V14" s="17"/>
       <c r="W14" s="113"/>
     </row>
-    <row r="15" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>42736</v>
       </c>
@@ -14120,31 +14151,31 @@
       <c r="V15" s="17"/>
       <c r="W15" s="113"/>
     </row>
-    <row r="16" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>42736</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>46</v>
+        <v>24</v>
+      </c>
+      <c r="D16" s="122" t="s">
+        <v>316</v>
+      </c>
+      <c r="E16" s="122" t="s">
+        <v>317</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="H16" s="122" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -14159,7 +14190,7 @@
       <c r="V16" s="17"/>
       <c r="W16" s="26"/>
     </row>
-    <row r="17" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>42736</v>
       </c>
@@ -14168,10 +14199,10 @@
         <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="3" t="s">
@@ -14183,7 +14214,7 @@
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -14198,7 +14229,7 @@
       <c r="V17" s="17"/>
       <c r="W17" s="26"/>
     </row>
-    <row r="18" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>42736</v>
       </c>
@@ -14207,20 +14238,22 @@
         <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -14235,7 +14268,7 @@
       <c r="V18" s="17"/>
       <c r="W18" s="26"/>
     </row>
-    <row r="19" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>42736</v>
       </c>
@@ -14244,14 +14277,14 @@
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -14272,7 +14305,7 @@
       <c r="V19" s="17"/>
       <c r="W19" s="26"/>
     </row>
-    <row r="20" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>42736</v>
       </c>
@@ -14281,20 +14314,20 @@
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -14309,7 +14342,7 @@
       <c r="V20" s="17"/>
       <c r="W20" s="26"/>
     </row>
-    <row r="21" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
         <v>42736</v>
       </c>
@@ -14318,14 +14351,14 @@
         <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -14346,7 +14379,7 @@
       <c r="V21" s="17"/>
       <c r="W21" s="26"/>
     </row>
-    <row r="22" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>42736</v>
       </c>
@@ -14355,20 +14388,20 @@
         <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -14383,7 +14416,7 @@
       <c r="V22" s="17"/>
       <c r="W22" s="26"/>
     </row>
-    <row r="23" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9">
         <v>42736</v>
       </c>
@@ -14392,20 +14425,20 @@
         <v>27</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -14420,7 +14453,7 @@
       <c r="V23" s="17"/>
       <c r="W23" s="26"/>
     </row>
-    <row r="24" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9">
         <v>42736</v>
       </c>
@@ -14429,20 +14462,20 @@
         <v>27</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="3" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -14457,7 +14490,7 @@
       <c r="V24" s="17"/>
       <c r="W24" s="26"/>
     </row>
-    <row r="25" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9">
         <v>42736</v>
       </c>
@@ -14466,22 +14499,20 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>88</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -14496,7 +14527,7 @@
       <c r="V25" s="17"/>
       <c r="W25" s="26"/>
     </row>
-    <row r="26" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9">
         <v>42736</v>
       </c>
@@ -14505,22 +14536,22 @@
         <v>27</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -14535,7 +14566,7 @@
       <c r="V26" s="17"/>
       <c r="W26" s="26"/>
     </row>
-    <row r="27" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9">
         <v>42736</v>
       </c>
@@ -14544,22 +14575,22 @@
         <v>27</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -14574,7 +14605,7 @@
       <c r="V27" s="17"/>
       <c r="W27" s="26"/>
     </row>
-    <row r="28" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9">
         <v>42736</v>
       </c>
@@ -14583,22 +14614,22 @@
         <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="3" t="s">
         <v>94</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -14613,18 +14644,32 @@
       <c r="V28" s="17"/>
       <c r="W28" s="26"/>
     </row>
-    <row r="29" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
+    <row r="29" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="9">
+        <v>42736</v>
+      </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="C29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="G29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -14638,7 +14683,7 @@
       <c r="V29" s="17"/>
       <c r="W29" s="26"/>
     </row>
-    <row r="30" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="4"/>
@@ -14663,7 +14708,7 @@
       <c r="V30" s="17"/>
       <c r="W30" s="26"/>
     </row>
-    <row r="31" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="4"/>
@@ -14688,7 +14733,7 @@
       <c r="V31" s="17"/>
       <c r="W31" s="26"/>
     </row>
-    <row r="32" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="4"/>
@@ -14713,7 +14758,7 @@
       <c r="V32" s="17"/>
       <c r="W32" s="26"/>
     </row>
-    <row r="33" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="4"/>
@@ -14738,7 +14783,7 @@
       <c r="V33" s="17"/>
       <c r="W33" s="26"/>
     </row>
-    <row r="34" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="4"/>
@@ -14763,7 +14808,7 @@
       <c r="V34" s="17"/>
       <c r="W34" s="26"/>
     </row>
-    <row r="35" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="4"/>
@@ -14788,7 +14833,7 @@
       <c r="V35" s="17"/>
       <c r="W35" s="26"/>
     </row>
-    <row r="36" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="4"/>
@@ -14813,7 +14858,7 @@
       <c r="V36" s="17"/>
       <c r="W36" s="26"/>
     </row>
-    <row r="37" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="4"/>
@@ -14838,7 +14883,7 @@
       <c r="V37" s="17"/>
       <c r="W37" s="26"/>
     </row>
-    <row r="38" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="4"/>
@@ -14857,11 +14902,36 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
-      <c r="S38" s="35"/>
-      <c r="T38" s="36"/>
-      <c r="U38" s="36"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="37"/>
+      <c r="S38" s="25"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="26"/>
+    </row>
+    <row r="39" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="35"/>
+      <c r="T39" s="36"/>
+      <c r="U39" s="36"/>
+      <c r="V39" s="36"/>
+      <c r="W39" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -14878,17 +14948,17 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.15234375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="31.69140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.3046875" style="1" customWidth="1"/>
-    <col min="6" max="10" width="8.84375" style="1" customWidth="1"/>
-    <col min="11" max="1025" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="31.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="1" customWidth="1"/>
+    <col min="6" max="10" width="8.83203125" style="1" customWidth="1"/>
+    <col min="11" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>97</v>
       </c>
@@ -14908,7 +14978,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -14926,7 +14996,7 @@
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -14948,7 +15018,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="38">
         <v>42736</v>
       </c>
@@ -14968,7 +15038,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="38">
         <v>42736</v>
       </c>
@@ -14988,7 +15058,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="38">
         <v>42736</v>
       </c>
@@ -15008,7 +15078,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="38">
         <v>42736</v>
       </c>
@@ -15028,7 +15098,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="38">
         <v>42736</v>
       </c>
@@ -15048,7 +15118,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="38">
         <v>42736</v>
       </c>
@@ -15068,7 +15138,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="38">
         <v>42736</v>
       </c>
@@ -15088,7 +15158,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="4"/>
@@ -15100,7 +15170,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="4"/>
@@ -15112,7 +15182,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="4"/>
@@ -15124,7 +15194,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="4"/>
@@ -15136,7 +15206,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="4"/>
@@ -15148,7 +15218,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="4"/>
@@ -15160,7 +15230,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="21"/>
       <c r="B17" s="9"/>
       <c r="C17" s="4"/>
@@ -15172,7 +15242,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="21"/>
       <c r="B18" s="9"/>
       <c r="C18" s="4"/>
@@ -15184,7 +15254,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="21"/>
       <c r="B19" s="9"/>
       <c r="C19" s="4"/>
@@ -15196,7 +15266,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="4"/>
@@ -15221,26 +15291,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21.69140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.4609375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.4609375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.69140625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="21.4609375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.84375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.15234375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.69140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="21.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="20" style="1" customWidth="1"/>
-    <col min="13" max="19" width="8.84375" style="1" customWidth="1"/>
-    <col min="20" max="1025" width="8.84375" customWidth="1"/>
+    <col min="13" max="19" width="8.83203125" style="1" customWidth="1"/>
+    <col min="20" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>115</v>
       </c>
@@ -15269,7 +15341,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -15310,7 +15382,7 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -15359,7 +15431,7 @@
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
     </row>
-    <row r="4" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -15392,7 +15464,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -15425,7 +15497,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -15458,7 +15530,7 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -15491,7 +15563,7 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
     </row>
-    <row r="8" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>42736</v>
       </c>
@@ -15526,7 +15598,7 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>42736</v>
       </c>
@@ -15559,7 +15631,7 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>42736</v>
       </c>
@@ -15592,7 +15664,7 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
     </row>
-    <row r="11" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>42736</v>
       </c>
@@ -15625,7 +15697,7 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
     </row>
-    <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>42736</v>
       </c>
@@ -15658,7 +15730,7 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>42736</v>
       </c>
@@ -15691,7 +15763,7 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>42736</v>
       </c>
@@ -15724,7 +15796,7 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>42736</v>
       </c>
@@ -15757,7 +15829,7 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
     </row>
-    <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>42736</v>
       </c>
@@ -15790,7 +15862,7 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>42736</v>
       </c>
@@ -15823,7 +15895,7 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>42736</v>
       </c>
@@ -15856,7 +15928,7 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>42736</v>
       </c>
@@ -15889,7 +15961,7 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>42736</v>
       </c>
@@ -15922,7 +15994,7 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
     </row>
-    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="21"/>
       <c r="B21" s="9"/>
       <c r="C21" s="4"/>
@@ -15943,7 +16015,7 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="4"/>
@@ -15964,7 +16036,7 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
     </row>
-    <row r="23" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="4"/>
@@ -15985,7 +16057,7 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9"/>
       <c r="B24" s="39"/>
       <c r="C24" s="4"/>
@@ -16006,7 +16078,7 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
-    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9"/>
       <c r="B25" s="21"/>
       <c r="C25" s="4"/>
@@ -16027,7 +16099,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9"/>
       <c r="B26" s="21"/>
       <c r="C26" s="4"/>
@@ -16048,7 +16120,7 @@
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
     </row>
-    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9"/>
       <c r="B27" s="21"/>
       <c r="C27" s="4"/>
@@ -16069,7 +16141,7 @@
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
     </row>
-    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9"/>
       <c r="B28" s="21"/>
       <c r="C28" s="4"/>
@@ -16090,7 +16162,7 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9"/>
       <c r="B29" s="21"/>
       <c r="C29" s="4"/>
@@ -16111,7 +16183,7 @@
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9"/>
       <c r="B30" s="21"/>
       <c r="C30" s="4"/>
@@ -16149,20 +16221,20 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.3046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.84375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.4609375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.69140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.69140625" style="1" customWidth="1"/>
-    <col min="8" max="12" width="8.84375" style="1" customWidth="1"/>
-    <col min="13" max="1025" width="8.84375" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8" max="12" width="8.83203125" style="1" customWidth="1"/>
+    <col min="13" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>142</v>
       </c>
@@ -16184,7 +16256,7 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -16200,7 +16272,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -16228,7 +16300,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -16252,7 +16324,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -16276,7 +16348,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -16300,7 +16372,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -16324,7 +16396,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>42736</v>
       </c>
@@ -16348,7 +16420,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>42736</v>
       </c>
@@ -16372,7 +16444,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="4"/>
@@ -16386,7 +16458,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="4"/>
@@ -16400,7 +16472,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="4"/>
@@ -16414,7 +16486,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="8"/>
@@ -16428,7 +16500,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="8"/>
@@ -16442,7 +16514,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="8"/>
@@ -16456,7 +16528,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="8"/>
@@ -16470,7 +16542,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>
@@ -16484,7 +16556,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="8"/>
@@ -16498,7 +16570,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="4"/>
@@ -16529,33 +16601,33 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.69140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.84375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.69140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.69140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.4609375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.69140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.4609375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.69140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.69140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="45.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="32" style="1" customWidth="1"/>
-    <col min="12" max="12" width="31.4609375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="29.84375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26.69140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="29.3046875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.69140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="31.15234375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.84375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="1" customWidth="1"/>
     <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.69140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8.84375" style="1" customWidth="1"/>
-    <col min="22" max="1025" width="8.84375" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" style="1" customWidth="1"/>
+    <col min="22" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>154</v>
       </c>
@@ -16586,7 +16658,7 @@
       <c r="T1" s="101"/>
       <c r="U1" s="4"/>
     </row>
-    <row r="2" spans="1:21" ht="65.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -16645,7 +16717,7 @@
       </c>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -16708,7 +16780,7 @@
       </c>
       <c r="U3" s="8"/>
     </row>
-    <row r="4" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -16759,7 +16831,7 @@
       </c>
       <c r="U4" s="4"/>
     </row>
-    <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -16806,7 +16878,7 @@
       <c r="T5" s="101"/>
       <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -16849,7 +16921,7 @@
       <c r="T6" s="101"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -16892,7 +16964,7 @@
       <c r="T7" s="101"/>
       <c r="U7" s="4"/>
     </row>
-    <row r="8" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>42736</v>
       </c>
@@ -16937,7 +17009,7 @@
       <c r="T8" s="101"/>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>42736</v>
       </c>
@@ -16980,7 +17052,7 @@
       <c r="T9" s="101"/>
       <c r="U9" s="4"/>
     </row>
-    <row r="10" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="4"/>
@@ -17003,7 +17075,7 @@
       <c r="T10" s="101"/>
       <c r="U10" s="4"/>
     </row>
-    <row r="11" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="4"/>
@@ -17026,7 +17098,7 @@
       <c r="T11" s="101"/>
       <c r="U11" s="4"/>
     </row>
-    <row r="12" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="4"/>
@@ -17049,7 +17121,7 @@
       <c r="T12" s="101"/>
       <c r="U12" s="4"/>
     </row>
-    <row r="13" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="4"/>
@@ -17072,7 +17144,7 @@
       <c r="T13" s="101"/>
       <c r="U13" s="4"/>
     </row>
-    <row r="14" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="4"/>
@@ -17095,7 +17167,7 @@
       <c r="T14" s="101"/>
       <c r="U14" s="4"/>
     </row>
-    <row r="15" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="4"/>
@@ -17118,7 +17190,7 @@
       <c r="T15" s="101"/>
       <c r="U15" s="4"/>
     </row>
-    <row r="16" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="4"/>
@@ -17141,7 +17213,7 @@
       <c r="T16" s="101"/>
       <c r="U16" s="4"/>
     </row>
-    <row r="17" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="4"/>
@@ -17164,7 +17236,7 @@
       <c r="T17" s="101"/>
       <c r="U17" s="4"/>
     </row>
-    <row r="18" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="4"/>
@@ -17187,7 +17259,7 @@
       <c r="T18" s="101"/>
       <c r="U18" s="4"/>
     </row>
-    <row r="19" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="4"/>
@@ -17221,32 +17293,32 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22.69140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.69140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.69140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.4609375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.84375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.4609375" style="1" customWidth="1"/>
-    <col min="10" max="11" width="20.15234375" style="1" customWidth="1"/>
-    <col min="12" max="13" width="22" style="1" customWidth="1"/>
-    <col min="14" max="14" width="45.3046875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="34.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="1024" width="8.84375" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="1" customWidth="1"/>
+    <col min="7" max="8" width="17.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5" style="1" customWidth="1"/>
+    <col min="10" max="12" width="20.1640625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="22" style="1" customWidth="1"/>
+    <col min="15" max="15" width="45.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -17266,14 +17338,15 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="101"/>
-      <c r="L1" s="4"/>
+      <c r="L1" s="101"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -17301,22 +17374,23 @@
       <c r="K2" s="102" t="s">
         <v>264</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="158"/>
+      <c r="M2" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="O2" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="O2" s="107" t="s">
+      <c r="P2" s="107" t="s">
         <v>274</v>
       </c>
-      <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
-    </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -17350,26 +17424,29 @@
       <c r="K3" s="103" t="s">
         <v>265</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="159" t="s">
+        <v>315</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="P3" s="156" t="s">
+      <c r="Q3" s="156" t="s">
         <v>309</v>
       </c>
-      <c r="Q3" s="156" t="s">
+      <c r="R3" s="156" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -17399,22 +17476,23 @@
       <c r="K4" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="101"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <v>2</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -17444,16 +17522,17 @@
       <c r="K5" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L5" s="4"/>
+      <c r="L5" s="101"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4">
+      <c r="O5" s="4"/>
+      <c r="P5" s="4">
         <v>1</v>
       </c>
-      <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -17483,16 +17562,17 @@
       <c r="K6" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="101"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="4"/>
+      <c r="O6" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -17518,16 +17598,17 @@
       <c r="K7" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="101"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="4"/>
+      <c r="O7" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>42736</v>
       </c>
@@ -17553,16 +17634,17 @@
       <c r="K8" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="101"/>
+      <c r="M8" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="4"/>
+      <c r="N8" s="3"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>42736</v>
       </c>
@@ -17592,14 +17674,15 @@
       <c r="K9" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="101"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="3"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="114">
         <v>42736</v>
       </c>
@@ -17631,14 +17714,15 @@
       </c>
       <c r="L10" s="118"/>
       <c r="M10" s="118"/>
-      <c r="N10" s="116" t="s">
+      <c r="N10" s="118"/>
+      <c r="O10" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="O10" s="118"/>
-      <c r="P10" s="101"/>
+      <c r="P10" s="118"/>
       <c r="Q10" s="101"/>
-    </row>
-    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R10" s="101"/>
+    </row>
+    <row r="11" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="114">
         <v>42736</v>
       </c>
@@ -17670,14 +17754,15 @@
       </c>
       <c r="L11" s="118"/>
       <c r="M11" s="118"/>
-      <c r="N11" s="116" t="s">
+      <c r="N11" s="118"/>
+      <c r="O11" s="116" t="s">
         <v>176</v>
       </c>
-      <c r="O11" s="118"/>
-      <c r="P11" s="101"/>
+      <c r="P11" s="118"/>
       <c r="Q11" s="101"/>
-    </row>
-    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R11" s="101"/>
+    </row>
+    <row r="12" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>42736</v>
       </c>
@@ -17709,20 +17794,21 @@
       <c r="K12" s="101" t="s">
         <v>195</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3" t="s">
+      <c r="L12" s="101"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="R12" s="4" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>42736</v>
       </c>
@@ -17754,40 +17840,41 @@
       <c r="K13" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="3" t="s">
+      <c r="L13" s="101"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-    </row>
-    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>42736</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>212</v>
+      <c r="E14" s="116" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14" s="122" t="s">
+        <v>317</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="3" t="s">
-        <v>81</v>
+      <c r="I14" s="122" t="s">
+        <v>316</v>
       </c>
       <c r="J14" s="4">
         <v>1</v>
@@ -17795,54 +17882,77 @@
       <c r="K14" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="L14" s="4"/>
+      <c r="L14" s="160" t="s">
+        <v>319</v>
+      </c>
       <c r="M14" s="4"/>
-      <c r="N14" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-    </row>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
+        <v>42736</v>
+      </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="4"/>
+      <c r="I15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="101" t="s">
+        <v>267</v>
+      </c>
+      <c r="L15" s="101"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="O15" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="122"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="122"/>
       <c r="J16" s="4"/>
       <c r="K16" s="101"/>
-      <c r="L16" s="4"/>
+      <c r="L16" s="160"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="4"/>
@@ -17854,14 +17964,15 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="101"/>
-      <c r="L17" s="4"/>
+      <c r="L17" s="101"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="4"/>
@@ -17873,17 +17984,18 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="101"/>
-      <c r="L18" s="4"/>
+      <c r="L18" s="101"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -17892,12 +18004,33 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="101"/>
-      <c r="L19" s="4"/>
+      <c r="L19" s="101"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="20" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="101"/>
+      <c r="L20" s="101"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -17916,18 +18049,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.84375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.84375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.84375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.15234375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.3046875" style="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.84375" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>213</v>
       </c>
@@ -17943,7 +18076,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" spans="1:6" ht="43.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.15">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="49" t="s">
@@ -17959,7 +18092,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="50" t="s">
         <v>7</v>
       </c>
@@ -17979,7 +18112,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
         <v>42736</v>
       </c>
@@ -17997,7 +18130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52">
         <v>42736</v>
       </c>
@@ -18015,7 +18148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52">
         <v>42736</v>
       </c>
@@ -18033,7 +18166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52">
         <v>42736</v>
       </c>
@@ -18051,7 +18184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52">
         <v>42736</v>
       </c>
@@ -18069,7 +18202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52">
         <v>42736</v>
       </c>
@@ -18087,7 +18220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52">
         <v>42736</v>
       </c>
@@ -18105,7 +18238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52">
         <v>42736</v>
       </c>
@@ -18123,7 +18256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52">
         <v>42736</v>
       </c>
@@ -18141,7 +18274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52">
         <v>42736</v>
       </c>
@@ -18159,7 +18292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52">
         <v>42736</v>
       </c>
@@ -18177,7 +18310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52">
         <v>42736</v>
       </c>
@@ -18195,7 +18328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52">
         <v>42736</v>
       </c>

</xml_diff>